<commit_message>
feat: Implement archived requisitions and material image viewing; fix: input field behavior and batch script path
</commit_message>
<xml_diff>
--- a/auto_upload/order_models/成品入庫TECO狀態.XLSX
+++ b/auto_upload/order_models/成品入庫TECO狀態.XLSX
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfpap\-\auto_upload\order_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfpap\june\auto_upload\order_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F31C69-0DB1-4D44-A5F1-DBA88B11DC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7869C9F-4571-43CE-88F1-171228AF5BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="216">
   <si>
     <t>ZP01</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>MVP-10_X=1050, Y=530, Z=630</t>
-  </si>
-  <si>
-    <t>100003057</t>
   </si>
   <si>
     <t>100003170</t>
@@ -1083,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1104,40 +1101,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1145,19 +1142,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>195</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>196</v>
-      </c>
-      <c r="F2" t="s">
-        <v>197</v>
       </c>
       <c r="G2" s="3">
         <v>44902</v>
@@ -1169,7 +1166,7 @@
         <v>45077</v>
       </c>
       <c r="J2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
@@ -1373,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1449,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -1473,7 +1470,7 @@
         <v>45456</v>
       </c>
       <c r="J10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K10" t="s">
         <v>1</v>
@@ -1487,19 +1484,19 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>200</v>
       </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>201</v>
-      </c>
-      <c r="F11" t="s">
-        <v>202</v>
       </c>
       <c r="G11" s="3">
         <v>45461</v>
@@ -1511,7 +1508,7 @@
         <v>45532</v>
       </c>
       <c r="J11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K11" t="s">
         <v>1</v>
@@ -1829,37 +1826,37 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>202</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="G20" s="3">
-        <v>45593</v>
+        <v>45645</v>
       </c>
       <c r="H20" s="3">
-        <v>45624</v>
+        <v>45645</v>
       </c>
       <c r="I20" s="3">
-        <v>45915</v>
+        <v>45681</v>
       </c>
       <c r="J20" t="s">
-        <v>2</v>
+        <v>197</v>
       </c>
       <c r="K20" t="s">
         <v>1</v>
       </c>
       <c r="L20" s="3">
-        <v>45589</v>
+        <v>45645</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1867,37 +1864,37 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
       </c>
       <c r="D21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="G21" s="3">
-        <v>45645</v>
+        <v>45681</v>
       </c>
       <c r="H21" s="3">
-        <v>45645</v>
+        <v>45769</v>
       </c>
       <c r="I21" s="3">
-        <v>45681</v>
+        <v>45912</v>
       </c>
       <c r="J21" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="K21" t="s">
         <v>1</v>
       </c>
       <c r="L21" s="3">
-        <v>45645</v>
+        <v>45679</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1905,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -1914,19 +1911,19 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G22" s="3">
-        <v>45681</v>
+        <v>45700</v>
       </c>
       <c r="H22" s="3">
-        <v>45769</v>
+        <v>45740</v>
       </c>
       <c r="I22" s="3">
-        <v>45912</v>
+        <v>45896</v>
       </c>
       <c r="J22" t="s">
         <v>14</v>
@@ -1935,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="3">
-        <v>45679</v>
+        <v>45698</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1943,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
@@ -1952,19 +1949,19 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G23" s="3">
         <v>45700</v>
       </c>
       <c r="H23" s="3">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="I23" s="3">
-        <v>45896</v>
+        <v>45868</v>
       </c>
       <c r="J23" t="s">
         <v>14</v>
@@ -1981,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
@@ -1990,19 +1987,19 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G24" s="3">
-        <v>45700</v>
+        <v>45755</v>
       </c>
       <c r="H24" s="3">
-        <v>45741</v>
+        <v>45898</v>
       </c>
       <c r="I24" s="3">
-        <v>45868</v>
+        <v>45987</v>
       </c>
       <c r="J24" t="s">
         <v>14</v>
@@ -2011,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="3">
-        <v>45698</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2019,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -2028,28 +2025,28 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="G25" s="3">
-        <v>45755</v>
+        <v>45762</v>
       </c>
       <c r="H25" s="3">
-        <v>45898</v>
+        <v>45796</v>
       </c>
       <c r="I25" s="3">
-        <v>45987</v>
+        <v>45947</v>
       </c>
       <c r="J25" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K25" t="s">
         <v>1</v>
       </c>
       <c r="L25" s="3">
-        <v>45748</v>
+        <v>45761</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2066,19 +2063,19 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="G26" s="3">
         <v>45762</v>
       </c>
       <c r="H26" s="3">
-        <v>45796</v>
+        <v>45863</v>
       </c>
       <c r="I26" s="3">
-        <v>45947</v>
+        <v>45910</v>
       </c>
       <c r="J26" t="s">
         <v>2</v>
@@ -2095,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -2104,19 +2101,19 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G27" s="3">
-        <v>45762</v>
+        <v>45779</v>
       </c>
       <c r="H27" s="3">
-        <v>45863</v>
+        <v>45880</v>
       </c>
       <c r="I27" s="3">
-        <v>45910</v>
+        <v>45916</v>
       </c>
       <c r="J27" t="s">
         <v>2</v>
@@ -2125,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="3">
-        <v>45761</v>
+        <v>45777</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2133,19 +2130,19 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>57</v>
-      </c>
-      <c r="F28" t="s">
-        <v>58</v>
       </c>
       <c r="G28" s="3">
         <v>45779</v>
@@ -2180,19 +2177,19 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G29" s="3">
-        <v>45779</v>
+        <v>45786</v>
       </c>
       <c r="H29" s="3">
-        <v>45880</v>
+        <v>45800</v>
       </c>
       <c r="I29" s="3">
-        <v>45916</v>
+        <v>45915</v>
       </c>
       <c r="J29" t="s">
         <v>2</v>
@@ -2201,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="3">
-        <v>45777</v>
+        <v>45782</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2209,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -2218,19 +2215,19 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="F30" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="G30" s="3">
-        <v>45786</v>
+        <v>45784</v>
       </c>
       <c r="H30" s="3">
-        <v>45800</v>
+        <v>45827</v>
       </c>
       <c r="I30" s="3">
-        <v>45915</v>
+        <v>45895</v>
       </c>
       <c r="J30" t="s">
         <v>2</v>
@@ -2256,19 +2253,19 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="G31" s="3">
-        <v>45784</v>
+        <v>45793</v>
       </c>
       <c r="H31" s="3">
         <v>45827</v>
       </c>
       <c r="I31" s="3">
-        <v>45895</v>
+        <v>45908</v>
       </c>
       <c r="J31" t="s">
         <v>2</v>
@@ -2277,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="3">
-        <v>45782</v>
+        <v>45789</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2285,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
@@ -2294,28 +2291,28 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F32" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G32" s="3">
-        <v>45793</v>
+        <v>45796</v>
       </c>
       <c r="H32" s="3">
-        <v>45827</v>
+        <v>45821</v>
       </c>
       <c r="I32" s="3">
-        <v>45908</v>
+        <v>45931</v>
       </c>
       <c r="J32" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="K32" t="s">
         <v>1</v>
       </c>
       <c r="L32" s="3">
-        <v>45789</v>
+        <v>45796</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2323,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -2332,22 +2329,22 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="G33" s="3">
-        <v>45796</v>
+        <v>45798</v>
       </c>
       <c r="H33" s="3">
-        <v>45821</v>
+        <v>45826</v>
       </c>
       <c r="I33" s="3">
-        <v>45931</v>
+        <v>45924</v>
       </c>
       <c r="J33" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="K33" t="s">
         <v>1</v>
@@ -2370,19 +2367,19 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="G34" s="3">
         <v>45798</v>
       </c>
       <c r="H34" s="3">
-        <v>45826</v>
+        <v>45799</v>
       </c>
       <c r="I34" s="3">
-        <v>45924</v>
+        <v>45909</v>
       </c>
       <c r="J34" t="s">
         <v>2</v>
@@ -2391,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="L34" s="3">
-        <v>45796</v>
+        <v>45797</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2399,7 +2396,7 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
@@ -2408,28 +2405,28 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F35" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G35" s="3">
-        <v>45798</v>
+        <v>45799</v>
       </c>
       <c r="H35" s="3">
+        <v>45817</v>
+      </c>
+      <c r="I35" s="3">
+        <v>45924</v>
+      </c>
+      <c r="J35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="3">
         <v>45799</v>
-      </c>
-      <c r="I35" s="3">
-        <v>45909</v>
-      </c>
-      <c r="J35" t="s">
-        <v>2</v>
-      </c>
-      <c r="K35" t="s">
-        <v>1</v>
-      </c>
-      <c r="L35" s="3">
-        <v>45797</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2437,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
@@ -2446,28 +2443,28 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G36" s="3">
-        <v>45799</v>
+        <v>45800</v>
       </c>
       <c r="H36" s="3">
-        <v>45817</v>
+        <v>45812</v>
       </c>
       <c r="I36" s="3">
-        <v>45924</v>
+        <v>45896</v>
       </c>
       <c r="J36" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K36" t="s">
         <v>1</v>
       </c>
       <c r="L36" s="3">
-        <v>45799</v>
+        <v>45800</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2475,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
@@ -2484,28 +2481,28 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G37" s="3">
-        <v>45800</v>
+        <v>45804</v>
       </c>
       <c r="H37" s="3">
-        <v>45812</v>
+        <v>45923</v>
       </c>
       <c r="I37" s="3">
-        <v>45896</v>
+        <v>46013</v>
       </c>
       <c r="J37" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K37" t="s">
         <v>1</v>
       </c>
       <c r="L37" s="3">
-        <v>45800</v>
+        <v>45804</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2513,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
@@ -2522,28 +2519,28 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F38" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G38" s="3">
-        <v>45804</v>
+        <v>45810</v>
       </c>
       <c r="H38" s="3">
-        <v>45923</v>
+        <v>45848</v>
       </c>
       <c r="I38" s="3">
-        <v>46013</v>
+        <v>45912</v>
       </c>
       <c r="J38" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K38" t="s">
         <v>1</v>
       </c>
       <c r="L38" s="3">
-        <v>45804</v>
+        <v>45806</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2551,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C39" s="2">
         <v>1</v>
@@ -2560,19 +2557,19 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="G39" s="3">
         <v>45810</v>
       </c>
       <c r="H39" s="3">
-        <v>45848</v>
+        <v>45853</v>
       </c>
       <c r="I39" s="3">
-        <v>45912</v>
+        <v>45915</v>
       </c>
       <c r="J39" t="s">
         <v>2</v>
@@ -2598,28 +2595,28 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="F40" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="G40" s="3">
-        <v>45810</v>
+        <v>45811</v>
       </c>
       <c r="H40" s="3">
-        <v>45853</v>
+        <v>45979</v>
       </c>
       <c r="I40" s="3">
-        <v>45915</v>
+        <v>46014</v>
       </c>
       <c r="J40" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="K40" t="s">
         <v>1</v>
       </c>
       <c r="L40" s="3">
-        <v>45806</v>
+        <v>45811</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2627,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
@@ -2636,22 +2633,22 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F41" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G41" s="3">
         <v>45811</v>
       </c>
       <c r="H41" s="3">
-        <v>45979</v>
+        <v>45821</v>
       </c>
       <c r="I41" s="3">
-        <v>46014</v>
+        <v>45910</v>
       </c>
       <c r="J41" t="s">
-        <v>91</v>
+        <v>2</v>
       </c>
       <c r="K41" t="s">
         <v>1</v>
@@ -2665,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C42" s="2">
         <v>1</v>
@@ -2674,22 +2671,22 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F42" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G42" s="3">
         <v>45811</v>
       </c>
       <c r="H42" s="3">
-        <v>45821</v>
+        <v>45820</v>
       </c>
       <c r="I42" s="3">
-        <v>45910</v>
+        <v>45978</v>
       </c>
       <c r="J42" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="K42" t="s">
         <v>1</v>
@@ -2703,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -2712,22 +2709,22 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F43" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G43" s="3">
         <v>45811</v>
       </c>
       <c r="H43" s="3">
-        <v>45820</v>
+        <v>45812</v>
       </c>
       <c r="I43" s="3">
-        <v>45978</v>
+        <v>45926</v>
       </c>
       <c r="J43" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="K43" t="s">
         <v>1</v>
@@ -2741,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
@@ -2750,19 +2747,19 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G44" s="3">
         <v>45811</v>
       </c>
       <c r="H44" s="3">
-        <v>45812</v>
+        <v>45860</v>
       </c>
       <c r="I44" s="3">
-        <v>45926</v>
+        <v>45904</v>
       </c>
       <c r="J44" t="s">
         <v>2</v>
@@ -2779,7 +2776,7 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C45" s="2">
         <v>1</v>
@@ -2788,19 +2785,19 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="F45" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="G45" s="3">
-        <v>45811</v>
+        <v>45813</v>
       </c>
       <c r="H45" s="3">
-        <v>45860</v>
+        <v>45814</v>
       </c>
       <c r="I45" s="3">
-        <v>45904</v>
+        <v>45896</v>
       </c>
       <c r="J45" t="s">
         <v>2</v>
@@ -2809,7 +2806,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="3">
-        <v>45811</v>
+        <v>45812</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2826,19 +2823,19 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="F46" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="G46" s="3">
         <v>45813</v>
       </c>
       <c r="H46" s="3">
-        <v>45814</v>
+        <v>45827</v>
       </c>
       <c r="I46" s="3">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="J46" t="s">
         <v>2</v>
@@ -2855,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C47" s="2">
         <v>1</v>
@@ -2864,19 +2861,19 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F47" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G47" s="3">
-        <v>45813</v>
+        <v>45824</v>
       </c>
       <c r="H47" s="3">
-        <v>45827</v>
+        <v>45912</v>
       </c>
       <c r="I47" s="3">
-        <v>45897</v>
+        <v>45994</v>
       </c>
       <c r="J47" t="s">
         <v>2</v>
@@ -2885,7 +2882,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="3">
-        <v>45812</v>
+        <v>45824</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2893,7 +2890,7 @@
         <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C48" s="2">
         <v>1</v>
@@ -2902,19 +2899,19 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F48" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G48" s="3">
-        <v>45824</v>
+        <v>45833</v>
       </c>
       <c r="H48" s="3">
-        <v>45912</v>
+        <v>45839</v>
       </c>
       <c r="I48" s="3">
-        <v>45994</v>
+        <v>45908</v>
       </c>
       <c r="J48" t="s">
         <v>2</v>
@@ -2923,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="3">
-        <v>45824</v>
+        <v>45833</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2931,19 +2928,19 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
         <v>112</v>
       </c>
-      <c r="C49" s="2">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2">
-        <v>0</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>113</v>
-      </c>
-      <c r="F49" t="s">
-        <v>114</v>
       </c>
       <c r="G49" s="3">
         <v>45833</v>
@@ -2952,7 +2949,7 @@
         <v>45839</v>
       </c>
       <c r="I49" s="3">
-        <v>45908</v>
+        <v>45911</v>
       </c>
       <c r="J49" t="s">
         <v>2</v>
@@ -2978,19 +2975,19 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="F50" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="G50" s="3">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="H50" s="3">
-        <v>45839</v>
+        <v>45884</v>
       </c>
       <c r="I50" s="3">
-        <v>45911</v>
+        <v>45950</v>
       </c>
       <c r="J50" t="s">
         <v>2</v>
@@ -2999,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="L50" s="3">
-        <v>45833</v>
+        <v>45834</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3016,22 +3013,22 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="F51" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="G51" s="3">
         <v>45834</v>
       </c>
       <c r="H51" s="3">
-        <v>45884</v>
+        <v>45849</v>
       </c>
       <c r="I51" s="3">
-        <v>45950</v>
+        <v>45947</v>
       </c>
       <c r="J51" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K51" t="s">
         <v>1</v>
@@ -3045,31 +3042,31 @@
         <v>0</v>
       </c>
       <c r="B52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="2">
-        <v>1</v>
-      </c>
-      <c r="D52" s="2">
-        <v>0</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>118</v>
-      </c>
-      <c r="F52" t="s">
-        <v>119</v>
       </c>
       <c r="G52" s="3">
         <v>45834</v>
       </c>
       <c r="H52" s="3">
-        <v>45849</v>
+        <v>45905</v>
       </c>
       <c r="I52" s="3">
-        <v>45947</v>
+        <v>45972</v>
       </c>
       <c r="J52" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K52" t="s">
         <v>1</v>
@@ -3092,19 +3089,19 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F53" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G53" s="3">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="H53" s="3">
-        <v>45905</v>
+        <v>45853</v>
       </c>
       <c r="I53" s="3">
-        <v>45972</v>
+        <v>45901</v>
       </c>
       <c r="J53" t="s">
         <v>2</v>
@@ -3113,7 +3110,7 @@
         <v>1</v>
       </c>
       <c r="L53" s="3">
-        <v>45834</v>
+        <v>45835</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3121,31 +3118,31 @@
         <v>0</v>
       </c>
       <c r="B54" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
         <v>121</v>
       </c>
-      <c r="C54" s="2">
-        <v>1</v>
-      </c>
-      <c r="D54" s="2">
-        <v>0</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>122</v>
-      </c>
-      <c r="F54" t="s">
-        <v>123</v>
       </c>
       <c r="G54" s="3">
         <v>45835</v>
       </c>
       <c r="H54" s="3">
-        <v>45853</v>
+        <v>45933</v>
       </c>
       <c r="I54" s="3">
-        <v>45901</v>
+        <v>45972</v>
       </c>
       <c r="J54" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K54" t="s">
         <v>1</v>
@@ -3168,10 +3165,10 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
+        <v>121</v>
+      </c>
+      <c r="F55" t="s">
         <v>122</v>
-      </c>
-      <c r="F55" t="s">
-        <v>123</v>
       </c>
       <c r="G55" s="3">
         <v>45835</v>
@@ -3206,22 +3203,22 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
+        <v>121</v>
+      </c>
+      <c r="F56" t="s">
         <v>122</v>
-      </c>
-      <c r="F56" t="s">
-        <v>123</v>
       </c>
       <c r="G56" s="3">
         <v>45835</v>
       </c>
       <c r="H56" s="3">
-        <v>45933</v>
+        <v>45847</v>
       </c>
       <c r="I56" s="3">
-        <v>45972</v>
+        <v>45901</v>
       </c>
       <c r="J56" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K56" t="s">
         <v>1</v>
@@ -3244,28 +3241,28 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
       <c r="F57" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="G57" s="3">
-        <v>45835</v>
+        <v>45839</v>
       </c>
       <c r="H57" s="3">
-        <v>45847</v>
+        <v>45933</v>
       </c>
       <c r="I57" s="3">
-        <v>45901</v>
+        <v>45959</v>
       </c>
       <c r="J57" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="K57" t="s">
         <v>1</v>
       </c>
       <c r="L57" s="3">
-        <v>45835</v>
+        <v>45839</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3282,28 +3279,28 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="F58" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="G58" s="3">
-        <v>45839</v>
+        <v>45846</v>
       </c>
       <c r="H58" s="3">
-        <v>45933</v>
+        <v>45854</v>
       </c>
       <c r="I58" s="3">
-        <v>45959</v>
+        <v>45888</v>
       </c>
       <c r="J58" t="s">
-        <v>91</v>
+        <v>2</v>
       </c>
       <c r="K58" t="s">
         <v>1</v>
       </c>
       <c r="L58" s="3">
-        <v>45839</v>
+        <v>45846</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3320,19 +3317,19 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F59" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G59" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="H59" s="3">
-        <v>45854</v>
+        <v>45860</v>
       </c>
       <c r="I59" s="3">
-        <v>45888</v>
+        <v>45897</v>
       </c>
       <c r="J59" t="s">
         <v>2</v>
@@ -3341,7 +3338,7 @@
         <v>1</v>
       </c>
       <c r="L59" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -3367,10 +3364,10 @@
         <v>45847</v>
       </c>
       <c r="H60" s="3">
-        <v>45860</v>
+        <v>45849</v>
       </c>
       <c r="I60" s="3">
-        <v>45897</v>
+        <v>45894</v>
       </c>
       <c r="J60" t="s">
         <v>2</v>
@@ -3396,16 +3393,16 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="F61" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="G61" s="3">
         <v>45847</v>
       </c>
       <c r="H61" s="3">
-        <v>45849</v>
+        <v>45852</v>
       </c>
       <c r="I61" s="3">
         <v>45894</v>
@@ -3425,28 +3422,28 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="2">
-        <v>1</v>
-      </c>
-      <c r="D62" s="2">
-        <v>0</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>132</v>
-      </c>
-      <c r="F62" t="s">
-        <v>133</v>
       </c>
       <c r="G62" s="3">
         <v>45847</v>
       </c>
       <c r="H62" s="3">
-        <v>45852</v>
+        <v>45860</v>
       </c>
       <c r="I62" s="3">
-        <v>45894</v>
+        <v>45897</v>
       </c>
       <c r="J62" t="s">
         <v>2</v>
@@ -3472,19 +3469,19 @@
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F63" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G63" s="3">
         <v>45847</v>
       </c>
       <c r="H63" s="3">
-        <v>45860</v>
+        <v>45854</v>
       </c>
       <c r="I63" s="3">
-        <v>45897</v>
+        <v>45888</v>
       </c>
       <c r="J63" t="s">
         <v>2</v>
@@ -3501,19 +3498,19 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
         <v>135</v>
       </c>
-      <c r="C64" s="2">
-        <v>1</v>
-      </c>
-      <c r="D64" s="2">
-        <v>0</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>136</v>
-      </c>
-      <c r="F64" t="s">
-        <v>137</v>
       </c>
       <c r="G64" s="3">
         <v>45847</v>
@@ -3522,7 +3519,7 @@
         <v>45854</v>
       </c>
       <c r="I64" s="3">
-        <v>45888</v>
+        <v>45894</v>
       </c>
       <c r="J64" t="s">
         <v>2</v>
@@ -3548,28 +3545,28 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F65" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G65" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="H65" s="3">
-        <v>45854</v>
+        <v>46016</v>
       </c>
       <c r="I65" s="3">
-        <v>45894</v>
+        <v>46107</v>
       </c>
       <c r="J65" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K65" t="s">
         <v>1</v>
       </c>
       <c r="L65" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3577,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C66" s="2">
         <v>1</v>
@@ -3586,28 +3583,28 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F66" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G66" s="3">
-        <v>45848</v>
+        <v>45849</v>
       </c>
       <c r="H66" s="3">
-        <v>46016</v>
+        <v>45882</v>
       </c>
       <c r="I66" s="3">
-        <v>46107</v>
+        <v>45916</v>
       </c>
       <c r="J66" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K66" t="s">
         <v>1</v>
       </c>
       <c r="L66" s="3">
-        <v>45848</v>
+        <v>45849</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3615,28 +3612,28 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
         <v>142</v>
       </c>
-      <c r="C67" s="2">
-        <v>1</v>
-      </c>
-      <c r="D67" s="2">
-        <v>0</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>143</v>
-      </c>
-      <c r="F67" t="s">
-        <v>144</v>
       </c>
       <c r="G67" s="3">
         <v>45849</v>
       </c>
       <c r="H67" s="3">
-        <v>45882</v>
+        <v>45880</v>
       </c>
       <c r="I67" s="3">
-        <v>45916</v>
+        <v>45910</v>
       </c>
       <c r="J67" t="s">
         <v>2</v>
@@ -3662,19 +3659,19 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="F68" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="G68" s="3">
-        <v>45849</v>
+        <v>45852</v>
       </c>
       <c r="H68" s="3">
-        <v>45880</v>
+        <v>45867</v>
       </c>
       <c r="I68" s="3">
-        <v>45910</v>
+        <v>45922</v>
       </c>
       <c r="J68" t="s">
         <v>2</v>
@@ -3683,7 +3680,7 @@
         <v>1</v>
       </c>
       <c r="L68" s="3">
-        <v>45849</v>
+        <v>45852</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3700,28 +3697,28 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F69" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="G69" s="3">
-        <v>45852</v>
+        <v>45860</v>
       </c>
       <c r="H69" s="3">
-        <v>45867</v>
+        <v>45880</v>
       </c>
       <c r="I69" s="3">
-        <v>45922</v>
+        <v>45919</v>
       </c>
       <c r="J69" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="K69" t="s">
         <v>1</v>
       </c>
       <c r="L69" s="3">
-        <v>45852</v>
+        <v>45860</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3729,7 +3726,7 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C70" s="2">
         <v>1</v>
@@ -3738,28 +3735,28 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="F70" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="G70" s="3">
-        <v>45860</v>
+        <v>45861</v>
       </c>
       <c r="H70" s="3">
-        <v>45880</v>
+        <v>45887</v>
       </c>
       <c r="I70" s="3">
-        <v>45919</v>
+        <v>45926</v>
       </c>
       <c r="J70" t="s">
-        <v>148</v>
+        <v>2</v>
       </c>
       <c r="K70" t="s">
         <v>1</v>
       </c>
       <c r="L70" s="3">
-        <v>45860</v>
+        <v>45861</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3785,13 +3782,13 @@
         <v>45861</v>
       </c>
       <c r="H71" s="3">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="I71" s="3">
-        <v>45926</v>
+        <v>45912</v>
       </c>
       <c r="J71" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="K71" t="s">
         <v>1</v>
@@ -3814,22 +3811,22 @@
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>28</v>
+        <v>151</v>
       </c>
       <c r="F72" t="s">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="G72" s="3">
         <v>45861</v>
       </c>
       <c r="H72" s="3">
-        <v>45883</v>
+        <v>45996</v>
       </c>
       <c r="I72" s="3">
-        <v>45912</v>
+        <v>46085</v>
       </c>
       <c r="J72" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="K72" t="s">
         <v>1</v>
@@ -3843,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C73" s="2">
         <v>1</v>
@@ -3852,28 +3849,28 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="F73" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="G73" s="3">
-        <v>45861</v>
+        <v>45866</v>
       </c>
       <c r="H73" s="3">
-        <v>45996</v>
+        <v>45880</v>
       </c>
       <c r="I73" s="3">
-        <v>46085</v>
+        <v>45910</v>
       </c>
       <c r="J73" t="s">
-        <v>154</v>
+        <v>2</v>
       </c>
       <c r="K73" t="s">
         <v>1</v>
       </c>
       <c r="L73" s="3">
-        <v>45861</v>
+        <v>45866</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3890,28 +3887,28 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>136</v>
+        <v>12</v>
       </c>
       <c r="F74" t="s">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="G74" s="3">
-        <v>45866</v>
+        <v>45870</v>
       </c>
       <c r="H74" s="3">
-        <v>45880</v>
+        <v>45987</v>
       </c>
       <c r="I74" s="3">
-        <v>45910</v>
+        <v>46055</v>
       </c>
       <c r="J74" t="s">
-        <v>2</v>
+        <v>156</v>
       </c>
       <c r="K74" t="s">
         <v>1</v>
       </c>
       <c r="L74" s="3">
-        <v>45866</v>
+        <v>45870</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3919,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C75" s="2">
         <v>1</v>
@@ -3928,28 +3925,28 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F75" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G75" s="3">
-        <v>45870</v>
+        <v>45876</v>
       </c>
       <c r="H75" s="3">
-        <v>45987</v>
+        <v>45877</v>
       </c>
       <c r="I75" s="3">
-        <v>46055</v>
+        <v>45910</v>
       </c>
       <c r="J75" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="K75" t="s">
         <v>1</v>
       </c>
       <c r="L75" s="3">
-        <v>45870</v>
+        <v>45875</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3966,28 +3963,28 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F76" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G76" s="3">
         <v>45876</v>
       </c>
       <c r="H76" s="3">
-        <v>45877</v>
+        <v>45891</v>
       </c>
       <c r="I76" s="3">
-        <v>45910</v>
+        <v>45917</v>
       </c>
       <c r="J76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K76" t="s">
         <v>1</v>
       </c>
       <c r="L76" s="3">
-        <v>45875</v>
+        <v>45876</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -4004,22 +4001,22 @@
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>37</v>
+        <v>160</v>
       </c>
       <c r="F77" t="s">
-        <v>38</v>
+        <v>161</v>
       </c>
       <c r="G77" s="3">
         <v>45876</v>
       </c>
       <c r="H77" s="3">
-        <v>45891</v>
+        <v>45961</v>
       </c>
       <c r="I77" s="3">
-        <v>45917</v>
+        <v>45994</v>
       </c>
       <c r="J77" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="K77" t="s">
         <v>1</v>
@@ -4033,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
@@ -4042,28 +4039,28 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="F78" t="s">
-        <v>162</v>
+        <v>23</v>
       </c>
       <c r="G78" s="3">
-        <v>45876</v>
+        <v>45880</v>
       </c>
       <c r="H78" s="3">
-        <v>45961</v>
+        <v>45925</v>
       </c>
       <c r="I78" s="3">
-        <v>45994</v>
+        <v>46021</v>
       </c>
       <c r="J78" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="K78" t="s">
         <v>1</v>
       </c>
       <c r="L78" s="3">
-        <v>45876</v>
+        <v>45880</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -4080,22 +4077,22 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
       <c r="F79" t="s">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="G79" s="3">
         <v>45880</v>
       </c>
       <c r="H79" s="3">
-        <v>45925</v>
+        <v>45887</v>
       </c>
       <c r="I79" s="3">
-        <v>46021</v>
+        <v>45938</v>
       </c>
       <c r="J79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K79" t="s">
         <v>1</v>
@@ -4118,22 +4115,22 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>161</v>
+        <v>53</v>
       </c>
       <c r="F80" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="G80" s="3">
         <v>45880</v>
       </c>
       <c r="H80" s="3">
-        <v>45887</v>
+        <v>45888</v>
       </c>
       <c r="I80" s="3">
-        <v>45938</v>
+        <v>45922</v>
       </c>
       <c r="J80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K80" t="s">
         <v>1</v>
@@ -4156,28 +4153,28 @@
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="F81" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="G81" s="3">
-        <v>45880</v>
+        <v>45882</v>
       </c>
       <c r="H81" s="3">
-        <v>45888</v>
+        <v>45918</v>
       </c>
       <c r="I81" s="3">
-        <v>45922</v>
+        <v>45945</v>
       </c>
       <c r="J81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K81" t="s">
         <v>1</v>
       </c>
       <c r="L81" s="3">
-        <v>45880</v>
+        <v>45882</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -4194,22 +4191,22 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="F82" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="G82" s="3">
         <v>45882</v>
       </c>
       <c r="H82" s="3">
-        <v>45918</v>
+        <v>45896</v>
       </c>
       <c r="I82" s="3">
-        <v>45945</v>
+        <v>45923</v>
       </c>
       <c r="J82" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K82" t="s">
         <v>1</v>
@@ -4232,28 +4229,28 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>57</v>
+        <v>168</v>
       </c>
       <c r="F83" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="G83" s="3">
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="H83" s="3">
-        <v>45896</v>
+        <v>45930</v>
       </c>
       <c r="I83" s="3">
-        <v>45923</v>
+        <v>45959</v>
       </c>
       <c r="J83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K83" t="s">
         <v>1</v>
       </c>
       <c r="L83" s="3">
-        <v>45882</v>
+        <v>45884</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -4261,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C84" s="2">
         <v>1</v>
@@ -4270,22 +4267,22 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="F84" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="G84" s="3">
         <v>45884</v>
       </c>
       <c r="H84" s="3">
-        <v>45930</v>
+        <v>45971</v>
       </c>
       <c r="I84" s="3">
-        <v>45959</v>
+        <v>45994</v>
       </c>
       <c r="J84" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="K84" t="s">
         <v>1</v>
@@ -4308,10 +4305,10 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
+        <v>131</v>
+      </c>
+      <c r="F85" t="s">
         <v>132</v>
-      </c>
-      <c r="F85" t="s">
-        <v>133</v>
       </c>
       <c r="G85" s="3">
         <v>45884</v>
@@ -4323,7 +4320,7 @@
         <v>45994</v>
       </c>
       <c r="J85" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K85" t="s">
         <v>1</v>
@@ -4346,10 +4343,10 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
+        <v>131</v>
+      </c>
+      <c r="F86" t="s">
         <v>132</v>
-      </c>
-      <c r="F86" t="s">
-        <v>133</v>
       </c>
       <c r="G86" s="3">
         <v>45884</v>
@@ -4361,7 +4358,7 @@
         <v>45994</v>
       </c>
       <c r="J86" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K86" t="s">
         <v>1</v>
@@ -4384,10 +4381,10 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
+        <v>131</v>
+      </c>
+      <c r="F87" t="s">
         <v>132</v>
-      </c>
-      <c r="F87" t="s">
-        <v>133</v>
       </c>
       <c r="G87" s="3">
         <v>45884</v>
@@ -4399,7 +4396,7 @@
         <v>45994</v>
       </c>
       <c r="J87" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K87" t="s">
         <v>1</v>
@@ -4422,22 +4419,22 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
+        <v>131</v>
+      </c>
+      <c r="F88" t="s">
         <v>132</v>
-      </c>
-      <c r="F88" t="s">
-        <v>133</v>
       </c>
       <c r="G88" s="3">
         <v>45884</v>
       </c>
       <c r="H88" s="3">
-        <v>45971</v>
+        <v>45958</v>
       </c>
       <c r="I88" s="3">
-        <v>45994</v>
+        <v>45981</v>
       </c>
       <c r="J88" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K88" t="s">
         <v>1</v>
@@ -4460,10 +4457,10 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
+        <v>131</v>
+      </c>
+      <c r="F89" t="s">
         <v>132</v>
-      </c>
-      <c r="F89" t="s">
-        <v>133</v>
       </c>
       <c r="G89" s="3">
         <v>45884</v>
@@ -4475,7 +4472,7 @@
         <v>45981</v>
       </c>
       <c r="J89" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K89" t="s">
         <v>1</v>
@@ -4498,10 +4495,10 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
+        <v>131</v>
+      </c>
+      <c r="F90" t="s">
         <v>132</v>
-      </c>
-      <c r="F90" t="s">
-        <v>133</v>
       </c>
       <c r="G90" s="3">
         <v>45884</v>
@@ -4513,7 +4510,7 @@
         <v>45981</v>
       </c>
       <c r="J90" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K90" t="s">
         <v>1</v>
@@ -4536,10 +4533,10 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
+        <v>131</v>
+      </c>
+      <c r="F91" t="s">
         <v>132</v>
-      </c>
-      <c r="F91" t="s">
-        <v>133</v>
       </c>
       <c r="G91" s="3">
         <v>45884</v>
@@ -4551,7 +4548,7 @@
         <v>45981</v>
       </c>
       <c r="J91" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K91" t="s">
         <v>1</v>
@@ -4574,28 +4571,28 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="F92" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="G92" s="3">
-        <v>45884</v>
+        <v>45887</v>
       </c>
       <c r="H92" s="3">
-        <v>45958</v>
+        <v>45999</v>
       </c>
       <c r="I92" s="3">
-        <v>45981</v>
+        <v>46084</v>
       </c>
       <c r="J92" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="K92" t="s">
         <v>1</v>
       </c>
       <c r="L92" s="3">
-        <v>45884</v>
+        <v>45887</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -4603,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C93" s="2">
         <v>1</v>
@@ -4612,28 +4609,28 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>180</v>
+        <v>37</v>
       </c>
       <c r="F93" t="s">
-        <v>181</v>
+        <v>38</v>
       </c>
       <c r="G93" s="3">
-        <v>45887</v>
+        <v>45891</v>
       </c>
       <c r="H93" s="3">
-        <v>45999</v>
+        <v>45905</v>
       </c>
       <c r="I93" s="3">
-        <v>46084</v>
+        <v>45926</v>
       </c>
       <c r="J93" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K93" t="s">
         <v>1</v>
       </c>
       <c r="L93" s="3">
-        <v>45887</v>
+        <v>45890</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -4641,7 +4638,7 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C94" s="2">
         <v>1</v>
@@ -4650,28 +4647,28 @@
         <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>37</v>
+        <v>185</v>
       </c>
       <c r="F94" t="s">
-        <v>38</v>
+        <v>186</v>
       </c>
       <c r="G94" s="3">
         <v>45891</v>
       </c>
       <c r="H94" s="3">
-        <v>45905</v>
+        <v>45895</v>
       </c>
       <c r="I94" s="3">
-        <v>45926</v>
+        <v>45916</v>
       </c>
       <c r="J94" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="K94" t="s">
         <v>1</v>
       </c>
       <c r="L94" s="3">
-        <v>45890</v>
+        <v>45891</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -4679,31 +4676,31 @@
         <v>0</v>
       </c>
       <c r="B95" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="2">
+        <v>1</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0</v>
+      </c>
+      <c r="E95" t="s">
         <v>185</v>
       </c>
-      <c r="C95" s="2">
-        <v>1</v>
-      </c>
-      <c r="D95" s="2">
-        <v>0</v>
-      </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>186</v>
-      </c>
-      <c r="F95" t="s">
-        <v>187</v>
       </c>
       <c r="G95" s="3">
         <v>45891</v>
       </c>
       <c r="H95" s="3">
-        <v>45895</v>
+        <v>45891</v>
       </c>
       <c r="I95" s="3">
-        <v>45916</v>
+        <v>45915</v>
       </c>
       <c r="J95" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K95" t="s">
         <v>1</v>
@@ -4726,28 +4723,28 @@
         <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>186</v>
+        <v>25</v>
       </c>
       <c r="F96" t="s">
-        <v>187</v>
+        <v>26</v>
       </c>
       <c r="G96" s="3">
-        <v>45891</v>
+        <v>45901</v>
       </c>
       <c r="H96" s="3">
-        <v>45891</v>
+        <v>45902</v>
       </c>
       <c r="I96" s="3">
-        <v>45915</v>
+        <v>45931</v>
       </c>
       <c r="J96" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K96" t="s">
         <v>1</v>
       </c>
       <c r="L96" s="3">
-        <v>45891</v>
+        <v>45901</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -4764,22 +4761,22 @@
         <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F97" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G97" s="3">
         <v>45901</v>
       </c>
       <c r="H97" s="3">
-        <v>45902</v>
+        <v>45968</v>
       </c>
       <c r="I97" s="3">
-        <v>45931</v>
+        <v>45993</v>
       </c>
       <c r="J97" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="K97" t="s">
         <v>1</v>
@@ -4793,7 +4790,7 @@
         <v>0</v>
       </c>
       <c r="B98" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C98" s="2">
         <v>1</v>
@@ -4802,22 +4799,22 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="F98" t="s">
-        <v>5</v>
+        <v>193</v>
       </c>
       <c r="G98" s="3">
         <v>45901</v>
       </c>
       <c r="H98" s="3">
-        <v>45968</v>
+        <v>46055</v>
       </c>
       <c r="I98" s="3">
-        <v>45993</v>
+        <v>46140</v>
       </c>
       <c r="J98" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K98" t="s">
         <v>1</v>
@@ -4826,47 +4823,9 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>0</v>
-      </c>
-      <c r="B99" t="s">
-        <v>192</v>
-      </c>
-      <c r="C99" s="2">
-        <v>1</v>
-      </c>
-      <c r="D99" s="2">
-        <v>0</v>
-      </c>
-      <c r="E99" t="s">
-        <v>193</v>
-      </c>
-      <c r="F99" t="s">
-        <v>194</v>
-      </c>
-      <c r="G99" s="3">
-        <v>45901</v>
-      </c>
-      <c r="H99" s="3">
-        <v>46055</v>
-      </c>
-      <c r="I99" s="3">
-        <v>46140</v>
-      </c>
-      <c r="J99" t="s">
-        <v>191</v>
-      </c>
-      <c r="K99" t="s">
-        <v>1</v>
-      </c>
-      <c r="L99" s="3">
-        <v>45901</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L99">
-    <sortCondition ref="B2:B99"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L98">
+    <sortCondition ref="B2:B98"/>
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: Handle image archiving and sum quantities in auto-upload
</commit_message>
<xml_diff>
--- a/auto_upload/order_models/成品入庫TECO狀態.XLSX
+++ b/auto_upload/order_models/成品入庫TECO狀態.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfpap\june\auto_upload\order_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7869C9F-4571-43CE-88F1-171228AF5BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638E83FF-EB7E-4FE2-ACFC-F0F3A4DA1DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="215">
   <si>
     <t>ZP01</t>
   </si>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>REL  MSPT PCNF PRC  MANC MSCP RESA RMWB*</t>
-  </si>
-  <si>
-    <t>100003303</t>
   </si>
   <si>
     <t>100003306</t>
@@ -1080,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1101,40 +1098,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1142,19 +1139,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>195</v>
-      </c>
-      <c r="F2" t="s">
-        <v>196</v>
       </c>
       <c r="G2" s="3">
         <v>44902</v>
@@ -1166,7 +1163,7 @@
         <v>45077</v>
       </c>
       <c r="J2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
@@ -1370,7 +1367,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1446,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -1470,7 +1467,7 @@
         <v>45456</v>
       </c>
       <c r="J10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K10" t="s">
         <v>1</v>
@@ -1484,19 +1481,19 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>199</v>
       </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>200</v>
-      </c>
-      <c r="F11" t="s">
-        <v>201</v>
       </c>
       <c r="G11" s="3">
         <v>45461</v>
@@ -1508,7 +1505,7 @@
         <v>45532</v>
       </c>
       <c r="J11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K11" t="s">
         <v>1</v>
@@ -1826,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -1835,10 +1832,10 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" t="s">
         <v>88</v>
-      </c>
-      <c r="F20" t="s">
-        <v>89</v>
       </c>
       <c r="G20" s="3">
         <v>45645</v>
@@ -1850,7 +1847,7 @@
         <v>45681</v>
       </c>
       <c r="J20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K20" t="s">
         <v>1</v>
@@ -2329,19 +2326,19 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="G33" s="3">
         <v>45798</v>
       </c>
       <c r="H33" s="3">
-        <v>45826</v>
+        <v>45799</v>
       </c>
       <c r="I33" s="3">
-        <v>45924</v>
+        <v>45909</v>
       </c>
       <c r="J33" t="s">
         <v>2</v>
@@ -2350,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="L33" s="3">
-        <v>45796</v>
+        <v>45797</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2358,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -2367,28 +2364,28 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F34" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G34" s="3">
-        <v>45798</v>
+        <v>45799</v>
       </c>
       <c r="H34" s="3">
+        <v>45817</v>
+      </c>
+      <c r="I34" s="3">
+        <v>45924</v>
+      </c>
+      <c r="J34" t="s">
+        <v>14</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3">
         <v>45799</v>
-      </c>
-      <c r="I34" s="3">
-        <v>45909</v>
-      </c>
-      <c r="J34" t="s">
-        <v>2</v>
-      </c>
-      <c r="K34" t="s">
-        <v>1</v>
-      </c>
-      <c r="L34" s="3">
-        <v>45797</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2396,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
@@ -2405,28 +2402,28 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F35" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G35" s="3">
-        <v>45799</v>
+        <v>45800</v>
       </c>
       <c r="H35" s="3">
-        <v>45817</v>
+        <v>45812</v>
       </c>
       <c r="I35" s="3">
-        <v>45924</v>
+        <v>45896</v>
       </c>
       <c r="J35" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K35" t="s">
         <v>1</v>
       </c>
       <c r="L35" s="3">
-        <v>45799</v>
+        <v>45800</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2434,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
@@ -2443,28 +2440,28 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G36" s="3">
-        <v>45800</v>
+        <v>45804</v>
       </c>
       <c r="H36" s="3">
-        <v>45812</v>
+        <v>45923</v>
       </c>
       <c r="I36" s="3">
-        <v>45896</v>
+        <v>46013</v>
       </c>
       <c r="J36" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K36" t="s">
         <v>1</v>
       </c>
       <c r="L36" s="3">
-        <v>45800</v>
+        <v>45804</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2472,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
@@ -2481,28 +2478,28 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F37" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G37" s="3">
-        <v>45804</v>
+        <v>45810</v>
       </c>
       <c r="H37" s="3">
-        <v>45923</v>
+        <v>45848</v>
       </c>
       <c r="I37" s="3">
-        <v>46013</v>
+        <v>45912</v>
       </c>
       <c r="J37" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K37" t="s">
         <v>1</v>
       </c>
       <c r="L37" s="3">
-        <v>45804</v>
+        <v>45806</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2510,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
@@ -2519,19 +2516,19 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="G38" s="3">
         <v>45810</v>
       </c>
       <c r="H38" s="3">
-        <v>45848</v>
+        <v>45853</v>
       </c>
       <c r="I38" s="3">
-        <v>45912</v>
+        <v>45915</v>
       </c>
       <c r="J38" t="s">
         <v>2</v>
@@ -2557,28 +2554,28 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="G39" s="3">
-        <v>45810</v>
+        <v>45811</v>
       </c>
       <c r="H39" s="3">
-        <v>45853</v>
+        <v>45979</v>
       </c>
       <c r="I39" s="3">
-        <v>45915</v>
+        <v>46014</v>
       </c>
       <c r="J39" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="K39" t="s">
         <v>1</v>
       </c>
       <c r="L39" s="3">
-        <v>45806</v>
+        <v>45811</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2586,7 +2583,7 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C40" s="2">
         <v>1</v>
@@ -2595,22 +2592,22 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F40" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G40" s="3">
         <v>45811</v>
       </c>
       <c r="H40" s="3">
-        <v>45979</v>
+        <v>45821</v>
       </c>
       <c r="I40" s="3">
-        <v>46014</v>
+        <v>45910</v>
       </c>
       <c r="J40" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="K40" t="s">
         <v>1</v>
@@ -2624,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
@@ -2633,22 +2630,22 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F41" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G41" s="3">
         <v>45811</v>
       </c>
       <c r="H41" s="3">
-        <v>45821</v>
+        <v>45820</v>
       </c>
       <c r="I41" s="3">
-        <v>45910</v>
+        <v>45978</v>
       </c>
       <c r="J41" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="K41" t="s">
         <v>1</v>
@@ -2662,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C42" s="2">
         <v>1</v>
@@ -2671,22 +2668,22 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F42" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G42" s="3">
         <v>45811</v>
       </c>
       <c r="H42" s="3">
-        <v>45820</v>
+        <v>45812</v>
       </c>
       <c r="I42" s="3">
-        <v>45978</v>
+        <v>45926</v>
       </c>
       <c r="J42" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="K42" t="s">
         <v>1</v>
@@ -2700,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -2709,19 +2706,19 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F43" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G43" s="3">
         <v>45811</v>
       </c>
       <c r="H43" s="3">
-        <v>45812</v>
+        <v>45860</v>
       </c>
       <c r="I43" s="3">
-        <v>45926</v>
+        <v>45904</v>
       </c>
       <c r="J43" t="s">
         <v>2</v>
@@ -2738,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
@@ -2747,19 +2744,19 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="F44" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="G44" s="3">
-        <v>45811</v>
+        <v>45813</v>
       </c>
       <c r="H44" s="3">
-        <v>45860</v>
+        <v>45814</v>
       </c>
       <c r="I44" s="3">
-        <v>45904</v>
+        <v>45896</v>
       </c>
       <c r="J44" t="s">
         <v>2</v>
@@ -2768,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="L44" s="3">
-        <v>45811</v>
+        <v>45812</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2785,19 +2782,19 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="F45" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="G45" s="3">
         <v>45813</v>
       </c>
       <c r="H45" s="3">
-        <v>45814</v>
+        <v>45827</v>
       </c>
       <c r="I45" s="3">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="J45" t="s">
         <v>2</v>
@@ -2814,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C46" s="2">
         <v>1</v>
@@ -2823,19 +2820,19 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F46" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G46" s="3">
-        <v>45813</v>
+        <v>45824</v>
       </c>
       <c r="H46" s="3">
-        <v>45827</v>
+        <v>45912</v>
       </c>
       <c r="I46" s="3">
-        <v>45897</v>
+        <v>45994</v>
       </c>
       <c r="J46" t="s">
         <v>2</v>
@@ -2844,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="L46" s="3">
-        <v>45812</v>
+        <v>45824</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2852,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C47" s="2">
         <v>1</v>
@@ -2861,19 +2858,19 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G47" s="3">
-        <v>45824</v>
+        <v>45833</v>
       </c>
       <c r="H47" s="3">
-        <v>45912</v>
+        <v>45839</v>
       </c>
       <c r="I47" s="3">
-        <v>45994</v>
+        <v>45908</v>
       </c>
       <c r="J47" t="s">
         <v>2</v>
@@ -2882,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="3">
-        <v>45824</v>
+        <v>45833</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2890,19 +2887,19 @@
         <v>0</v>
       </c>
       <c r="B48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
         <v>111</v>
       </c>
-      <c r="C48" s="2">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2">
-        <v>0</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>112</v>
-      </c>
-      <c r="F48" t="s">
-        <v>113</v>
       </c>
       <c r="G48" s="3">
         <v>45833</v>
@@ -2911,7 +2908,7 @@
         <v>45839</v>
       </c>
       <c r="I48" s="3">
-        <v>45908</v>
+        <v>45911</v>
       </c>
       <c r="J48" t="s">
         <v>2</v>
@@ -2937,19 +2934,19 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="F49" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="G49" s="3">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="H49" s="3">
-        <v>45839</v>
+        <v>45884</v>
       </c>
       <c r="I49" s="3">
-        <v>45911</v>
+        <v>45950</v>
       </c>
       <c r="J49" t="s">
         <v>2</v>
@@ -2958,7 +2955,7 @@
         <v>1</v>
       </c>
       <c r="L49" s="3">
-        <v>45833</v>
+        <v>45834</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2975,22 +2972,22 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="F50" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="G50" s="3">
         <v>45834</v>
       </c>
       <c r="H50" s="3">
-        <v>45884</v>
+        <v>45849</v>
       </c>
       <c r="I50" s="3">
-        <v>45950</v>
+        <v>45947</v>
       </c>
       <c r="J50" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K50" t="s">
         <v>1</v>
@@ -3004,31 +3001,31 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
         <v>116</v>
       </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>117</v>
-      </c>
-      <c r="F51" t="s">
-        <v>118</v>
       </c>
       <c r="G51" s="3">
         <v>45834</v>
       </c>
       <c r="H51" s="3">
-        <v>45849</v>
+        <v>45905</v>
       </c>
       <c r="I51" s="3">
-        <v>45947</v>
+        <v>45972</v>
       </c>
       <c r="J51" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K51" t="s">
         <v>1</v>
@@ -3051,19 +3048,19 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F52" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G52" s="3">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="H52" s="3">
-        <v>45905</v>
+        <v>45853</v>
       </c>
       <c r="I52" s="3">
-        <v>45972</v>
+        <v>45901</v>
       </c>
       <c r="J52" t="s">
         <v>2</v>
@@ -3072,7 +3069,7 @@
         <v>1</v>
       </c>
       <c r="L52" s="3">
-        <v>45834</v>
+        <v>45835</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3080,31 +3077,31 @@
         <v>0</v>
       </c>
       <c r="B53" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
         <v>120</v>
       </c>
-      <c r="C53" s="2">
-        <v>1</v>
-      </c>
-      <c r="D53" s="2">
-        <v>0</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>121</v>
-      </c>
-      <c r="F53" t="s">
-        <v>122</v>
       </c>
       <c r="G53" s="3">
         <v>45835</v>
       </c>
       <c r="H53" s="3">
-        <v>45853</v>
+        <v>45933</v>
       </c>
       <c r="I53" s="3">
-        <v>45901</v>
+        <v>45972</v>
       </c>
       <c r="J53" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K53" t="s">
         <v>1</v>
@@ -3127,10 +3124,10 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" t="s">
         <v>121</v>
-      </c>
-      <c r="F54" t="s">
-        <v>122</v>
       </c>
       <c r="G54" s="3">
         <v>45835</v>
@@ -3165,22 +3162,22 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" t="s">
         <v>121</v>
-      </c>
-      <c r="F55" t="s">
-        <v>122</v>
       </c>
       <c r="G55" s="3">
         <v>45835</v>
       </c>
       <c r="H55" s="3">
-        <v>45933</v>
+        <v>45847</v>
       </c>
       <c r="I55" s="3">
-        <v>45972</v>
+        <v>45901</v>
       </c>
       <c r="J55" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K55" t="s">
         <v>1</v>
@@ -3203,28 +3200,28 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="F56" t="s">
-        <v>122</v>
+        <v>54</v>
       </c>
       <c r="G56" s="3">
-        <v>45835</v>
+        <v>45839</v>
       </c>
       <c r="H56" s="3">
-        <v>45847</v>
+        <v>45933</v>
       </c>
       <c r="I56" s="3">
-        <v>45901</v>
+        <v>45959</v>
       </c>
       <c r="J56" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="K56" t="s">
         <v>1</v>
       </c>
       <c r="L56" s="3">
-        <v>45835</v>
+        <v>45839</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3241,28 +3238,28 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="F57" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="G57" s="3">
-        <v>45839</v>
+        <v>45846</v>
       </c>
       <c r="H57" s="3">
-        <v>45933</v>
+        <v>45854</v>
       </c>
       <c r="I57" s="3">
-        <v>45959</v>
+        <v>45888</v>
       </c>
       <c r="J57" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="K57" t="s">
         <v>1</v>
       </c>
       <c r="L57" s="3">
-        <v>45839</v>
+        <v>45846</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3279,19 +3276,19 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F58" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G58" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="H58" s="3">
-        <v>45854</v>
+        <v>45860</v>
       </c>
       <c r="I58" s="3">
-        <v>45888</v>
+        <v>45897</v>
       </c>
       <c r="J58" t="s">
         <v>2</v>
@@ -3300,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="L58" s="3">
-        <v>45846</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3326,10 +3323,10 @@
         <v>45847</v>
       </c>
       <c r="H59" s="3">
-        <v>45860</v>
+        <v>45849</v>
       </c>
       <c r="I59" s="3">
-        <v>45897</v>
+        <v>45894</v>
       </c>
       <c r="J59" t="s">
         <v>2</v>
@@ -3355,16 +3352,16 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="F60" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="G60" s="3">
         <v>45847</v>
       </c>
       <c r="H60" s="3">
-        <v>45849</v>
+        <v>45852</v>
       </c>
       <c r="I60" s="3">
         <v>45894</v>
@@ -3384,28 +3381,28 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
         <v>130</v>
       </c>
-      <c r="C61" s="2">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2">
-        <v>0</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>131</v>
-      </c>
-      <c r="F61" t="s">
-        <v>132</v>
       </c>
       <c r="G61" s="3">
         <v>45847</v>
       </c>
       <c r="H61" s="3">
-        <v>45852</v>
+        <v>45860</v>
       </c>
       <c r="I61" s="3">
-        <v>45894</v>
+        <v>45897</v>
       </c>
       <c r="J61" t="s">
         <v>2</v>
@@ -3431,19 +3428,19 @@
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F62" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G62" s="3">
         <v>45847</v>
       </c>
       <c r="H62" s="3">
-        <v>45860</v>
+        <v>45854</v>
       </c>
       <c r="I62" s="3">
-        <v>45897</v>
+        <v>45888</v>
       </c>
       <c r="J62" t="s">
         <v>2</v>
@@ -3460,19 +3457,19 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
         <v>134</v>
       </c>
-      <c r="C63" s="2">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2">
-        <v>0</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>135</v>
-      </c>
-      <c r="F63" t="s">
-        <v>136</v>
       </c>
       <c r="G63" s="3">
         <v>45847</v>
@@ -3481,7 +3478,7 @@
         <v>45854</v>
       </c>
       <c r="I63" s="3">
-        <v>45888</v>
+        <v>45894</v>
       </c>
       <c r="J63" t="s">
         <v>2</v>
@@ -3507,28 +3504,28 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F64" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G64" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="H64" s="3">
-        <v>45854</v>
+        <v>46016</v>
       </c>
       <c r="I64" s="3">
-        <v>45894</v>
+        <v>46107</v>
       </c>
       <c r="J64" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K64" t="s">
         <v>1</v>
       </c>
       <c r="L64" s="3">
-        <v>45847</v>
+        <v>45848</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -3536,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C65" s="2">
         <v>1</v>
@@ -3545,28 +3542,28 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F65" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G65" s="3">
-        <v>45848</v>
+        <v>45849</v>
       </c>
       <c r="H65" s="3">
-        <v>46016</v>
+        <v>45882</v>
       </c>
       <c r="I65" s="3">
-        <v>46107</v>
+        <v>45916</v>
       </c>
       <c r="J65" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K65" t="s">
         <v>1</v>
       </c>
       <c r="L65" s="3">
-        <v>45848</v>
+        <v>45849</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3574,28 +3571,28 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
         <v>141</v>
       </c>
-      <c r="C66" s="2">
-        <v>1</v>
-      </c>
-      <c r="D66" s="2">
-        <v>0</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>142</v>
-      </c>
-      <c r="F66" t="s">
-        <v>143</v>
       </c>
       <c r="G66" s="3">
         <v>45849</v>
       </c>
       <c r="H66" s="3">
-        <v>45882</v>
+        <v>45880</v>
       </c>
       <c r="I66" s="3">
-        <v>45916</v>
+        <v>45910</v>
       </c>
       <c r="J66" t="s">
         <v>2</v>
@@ -3621,19 +3618,19 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="F67" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="G67" s="3">
-        <v>45849</v>
+        <v>45852</v>
       </c>
       <c r="H67" s="3">
-        <v>45880</v>
+        <v>45867</v>
       </c>
       <c r="I67" s="3">
-        <v>45910</v>
+        <v>45922</v>
       </c>
       <c r="J67" t="s">
         <v>2</v>
@@ -3642,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="L67" s="3">
-        <v>45849</v>
+        <v>45852</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3659,28 +3656,28 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="F68" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="G68" s="3">
-        <v>45852</v>
+        <v>45860</v>
       </c>
       <c r="H68" s="3">
-        <v>45867</v>
+        <v>45880</v>
       </c>
       <c r="I68" s="3">
-        <v>45922</v>
+        <v>45919</v>
       </c>
       <c r="J68" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
       <c r="K68" t="s">
         <v>1</v>
       </c>
       <c r="L68" s="3">
-        <v>45852</v>
+        <v>45860</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3688,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C69" s="2">
         <v>1</v>
@@ -3697,28 +3694,28 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="F69" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="G69" s="3">
-        <v>45860</v>
+        <v>45861</v>
       </c>
       <c r="H69" s="3">
-        <v>45880</v>
+        <v>45887</v>
       </c>
       <c r="I69" s="3">
-        <v>45919</v>
+        <v>45926</v>
       </c>
       <c r="J69" t="s">
-        <v>147</v>
+        <v>2</v>
       </c>
       <c r="K69" t="s">
         <v>1</v>
       </c>
       <c r="L69" s="3">
-        <v>45860</v>
+        <v>45861</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3744,13 +3741,13 @@
         <v>45861</v>
       </c>
       <c r="H70" s="3">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="I70" s="3">
-        <v>45926</v>
+        <v>45912</v>
       </c>
       <c r="J70" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
       <c r="K70" t="s">
         <v>1</v>
@@ -3773,22 +3770,22 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="F71" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="G71" s="3">
         <v>45861</v>
       </c>
       <c r="H71" s="3">
-        <v>45883</v>
+        <v>45996</v>
       </c>
       <c r="I71" s="3">
-        <v>45912</v>
+        <v>46085</v>
       </c>
       <c r="J71" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="K71" t="s">
         <v>1</v>
@@ -3802,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
@@ -3811,28 +3808,28 @@
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="F72" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="G72" s="3">
-        <v>45861</v>
+        <v>45866</v>
       </c>
       <c r="H72" s="3">
-        <v>45996</v>
+        <v>45880</v>
       </c>
       <c r="I72" s="3">
-        <v>46085</v>
+        <v>45910</v>
       </c>
       <c r="J72" t="s">
-        <v>153</v>
+        <v>2</v>
       </c>
       <c r="K72" t="s">
         <v>1</v>
       </c>
       <c r="L72" s="3">
-        <v>45861</v>
+        <v>45866</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -3849,28 +3846,28 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="F73" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="G73" s="3">
-        <v>45866</v>
+        <v>45870</v>
       </c>
       <c r="H73" s="3">
-        <v>45880</v>
+        <v>45987</v>
       </c>
       <c r="I73" s="3">
-        <v>45910</v>
+        <v>46055</v>
       </c>
       <c r="J73" t="s">
-        <v>2</v>
+        <v>155</v>
       </c>
       <c r="K73" t="s">
         <v>1</v>
       </c>
       <c r="L73" s="3">
-        <v>45866</v>
+        <v>45870</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3878,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C74" s="2">
         <v>1</v>
@@ -3887,28 +3884,28 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F74" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G74" s="3">
-        <v>45870</v>
+        <v>45876</v>
       </c>
       <c r="H74" s="3">
-        <v>45987</v>
+        <v>45877</v>
       </c>
       <c r="I74" s="3">
-        <v>46055</v>
+        <v>45910</v>
       </c>
       <c r="J74" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="K74" t="s">
         <v>1</v>
       </c>
       <c r="L74" s="3">
-        <v>45870</v>
+        <v>45875</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3925,28 +3922,28 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F75" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G75" s="3">
         <v>45876</v>
       </c>
       <c r="H75" s="3">
-        <v>45877</v>
+        <v>45891</v>
       </c>
       <c r="I75" s="3">
-        <v>45910</v>
+        <v>45917</v>
       </c>
       <c r="J75" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K75" t="s">
         <v>1</v>
       </c>
       <c r="L75" s="3">
-        <v>45875</v>
+        <v>45876</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3963,22 +3960,22 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="F76" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="G76" s="3">
         <v>45876</v>
       </c>
       <c r="H76" s="3">
-        <v>45891</v>
+        <v>45961</v>
       </c>
       <c r="I76" s="3">
-        <v>45917</v>
+        <v>45994</v>
       </c>
       <c r="J76" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="K76" t="s">
         <v>1</v>
@@ -3992,7 +3989,7 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C77" s="2">
         <v>1</v>
@@ -4001,28 +3998,28 @@
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="F77" t="s">
-        <v>161</v>
+        <v>23</v>
       </c>
       <c r="G77" s="3">
-        <v>45876</v>
+        <v>45880</v>
       </c>
       <c r="H77" s="3">
-        <v>45961</v>
+        <v>45925</v>
       </c>
       <c r="I77" s="3">
-        <v>45994</v>
+        <v>46021</v>
       </c>
       <c r="J77" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="K77" t="s">
         <v>1</v>
       </c>
       <c r="L77" s="3">
-        <v>45876</v>
+        <v>45880</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -4039,22 +4036,22 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="F78" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="G78" s="3">
         <v>45880</v>
       </c>
       <c r="H78" s="3">
-        <v>45925</v>
+        <v>45887</v>
       </c>
       <c r="I78" s="3">
-        <v>46021</v>
+        <v>45938</v>
       </c>
       <c r="J78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K78" t="s">
         <v>1</v>
@@ -4077,22 +4074,22 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="F79" t="s">
-        <v>161</v>
+        <v>54</v>
       </c>
       <c r="G79" s="3">
         <v>45880</v>
       </c>
       <c r="H79" s="3">
-        <v>45887</v>
+        <v>45888</v>
       </c>
       <c r="I79" s="3">
-        <v>45938</v>
+        <v>45922</v>
       </c>
       <c r="J79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K79" t="s">
         <v>1</v>
@@ -4115,28 +4112,28 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="F80" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="G80" s="3">
-        <v>45880</v>
+        <v>45882</v>
       </c>
       <c r="H80" s="3">
-        <v>45888</v>
+        <v>45918</v>
       </c>
       <c r="I80" s="3">
-        <v>45922</v>
+        <v>45945</v>
       </c>
       <c r="J80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K80" t="s">
         <v>1</v>
       </c>
       <c r="L80" s="3">
-        <v>45880</v>
+        <v>45882</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -4153,22 +4150,22 @@
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="F81" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="G81" s="3">
         <v>45882</v>
       </c>
       <c r="H81" s="3">
-        <v>45918</v>
+        <v>45896</v>
       </c>
       <c r="I81" s="3">
-        <v>45945</v>
+        <v>45923</v>
       </c>
       <c r="J81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K81" t="s">
         <v>1</v>
@@ -4191,28 +4188,28 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>56</v>
+        <v>167</v>
       </c>
       <c r="F82" t="s">
-        <v>57</v>
+        <v>168</v>
       </c>
       <c r="G82" s="3">
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="H82" s="3">
-        <v>45896</v>
+        <v>45930</v>
       </c>
       <c r="I82" s="3">
-        <v>45923</v>
+        <v>45959</v>
       </c>
       <c r="J82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K82" t="s">
         <v>1</v>
       </c>
       <c r="L82" s="3">
-        <v>45882</v>
+        <v>45884</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -4220,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C83" s="2">
         <v>1</v>
@@ -4229,22 +4226,22 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="F83" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="G83" s="3">
         <v>45884</v>
       </c>
       <c r="H83" s="3">
-        <v>45930</v>
+        <v>45971</v>
       </c>
       <c r="I83" s="3">
-        <v>45959</v>
+        <v>45994</v>
       </c>
       <c r="J83" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="K83" t="s">
         <v>1</v>
@@ -4267,10 +4264,10 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
+        <v>130</v>
+      </c>
+      <c r="F84" t="s">
         <v>131</v>
-      </c>
-      <c r="F84" t="s">
-        <v>132</v>
       </c>
       <c r="G84" s="3">
         <v>45884</v>
@@ -4282,7 +4279,7 @@
         <v>45994</v>
       </c>
       <c r="J84" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K84" t="s">
         <v>1</v>
@@ -4305,10 +4302,10 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
+        <v>130</v>
+      </c>
+      <c r="F85" t="s">
         <v>131</v>
-      </c>
-      <c r="F85" t="s">
-        <v>132</v>
       </c>
       <c r="G85" s="3">
         <v>45884</v>
@@ -4320,7 +4317,7 @@
         <v>45994</v>
       </c>
       <c r="J85" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K85" t="s">
         <v>1</v>
@@ -4343,10 +4340,10 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
+        <v>130</v>
+      </c>
+      <c r="F86" t="s">
         <v>131</v>
-      </c>
-      <c r="F86" t="s">
-        <v>132</v>
       </c>
       <c r="G86" s="3">
         <v>45884</v>
@@ -4358,7 +4355,7 @@
         <v>45994</v>
       </c>
       <c r="J86" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K86" t="s">
         <v>1</v>
@@ -4381,22 +4378,22 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
+        <v>130</v>
+      </c>
+      <c r="F87" t="s">
         <v>131</v>
-      </c>
-      <c r="F87" t="s">
-        <v>132</v>
       </c>
       <c r="G87" s="3">
         <v>45884</v>
       </c>
       <c r="H87" s="3">
-        <v>45971</v>
+        <v>45958</v>
       </c>
       <c r="I87" s="3">
-        <v>45994</v>
+        <v>45981</v>
       </c>
       <c r="J87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K87" t="s">
         <v>1</v>
@@ -4419,10 +4416,10 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
+        <v>130</v>
+      </c>
+      <c r="F88" t="s">
         <v>131</v>
-      </c>
-      <c r="F88" t="s">
-        <v>132</v>
       </c>
       <c r="G88" s="3">
         <v>45884</v>
@@ -4434,7 +4431,7 @@
         <v>45981</v>
       </c>
       <c r="J88" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K88" t="s">
         <v>1</v>
@@ -4457,10 +4454,10 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
+        <v>130</v>
+      </c>
+      <c r="F89" t="s">
         <v>131</v>
-      </c>
-      <c r="F89" t="s">
-        <v>132</v>
       </c>
       <c r="G89" s="3">
         <v>45884</v>
@@ -4472,7 +4469,7 @@
         <v>45981</v>
       </c>
       <c r="J89" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K89" t="s">
         <v>1</v>
@@ -4495,10 +4492,10 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
+        <v>130</v>
+      </c>
+      <c r="F90" t="s">
         <v>131</v>
-      </c>
-      <c r="F90" t="s">
-        <v>132</v>
       </c>
       <c r="G90" s="3">
         <v>45884</v>
@@ -4510,7 +4507,7 @@
         <v>45981</v>
       </c>
       <c r="J90" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K90" t="s">
         <v>1</v>
@@ -4533,28 +4530,28 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="F91" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="G91" s="3">
-        <v>45884</v>
+        <v>45887</v>
       </c>
       <c r="H91" s="3">
-        <v>45958</v>
+        <v>45999</v>
       </c>
       <c r="I91" s="3">
-        <v>45981</v>
+        <v>46084</v>
       </c>
       <c r="J91" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="K91" t="s">
         <v>1</v>
       </c>
       <c r="L91" s="3">
-        <v>45884</v>
+        <v>45887</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -4562,7 +4559,7 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C92" s="2">
         <v>1</v>
@@ -4571,28 +4568,28 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>179</v>
+        <v>37</v>
       </c>
       <c r="F92" t="s">
-        <v>180</v>
+        <v>38</v>
       </c>
       <c r="G92" s="3">
-        <v>45887</v>
+        <v>45891</v>
       </c>
       <c r="H92" s="3">
-        <v>45999</v>
+        <v>45905</v>
       </c>
       <c r="I92" s="3">
-        <v>46084</v>
+        <v>45926</v>
       </c>
       <c r="J92" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K92" t="s">
         <v>1</v>
       </c>
       <c r="L92" s="3">
-        <v>45887</v>
+        <v>45890</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -4600,7 +4597,7 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C93" s="2">
         <v>1</v>
@@ -4609,28 +4606,28 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>37</v>
+        <v>184</v>
       </c>
       <c r="F93" t="s">
-        <v>38</v>
+        <v>185</v>
       </c>
       <c r="G93" s="3">
         <v>45891</v>
       </c>
       <c r="H93" s="3">
-        <v>45905</v>
+        <v>45895</v>
       </c>
       <c r="I93" s="3">
-        <v>45926</v>
+        <v>45916</v>
       </c>
       <c r="J93" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="K93" t="s">
         <v>1</v>
       </c>
       <c r="L93" s="3">
-        <v>45890</v>
+        <v>45891</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -4638,31 +4635,31 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="2">
+        <v>1</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
         <v>184</v>
       </c>
-      <c r="C94" s="2">
-        <v>1</v>
-      </c>
-      <c r="D94" s="2">
-        <v>0</v>
-      </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>185</v>
-      </c>
-      <c r="F94" t="s">
-        <v>186</v>
       </c>
       <c r="G94" s="3">
         <v>45891</v>
       </c>
       <c r="H94" s="3">
-        <v>45895</v>
+        <v>45891</v>
       </c>
       <c r="I94" s="3">
-        <v>45916</v>
+        <v>45915</v>
       </c>
       <c r="J94" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K94" t="s">
         <v>1</v>
@@ -4685,28 +4682,28 @@
         <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="F95" t="s">
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="G95" s="3">
-        <v>45891</v>
+        <v>45901</v>
       </c>
       <c r="H95" s="3">
-        <v>45891</v>
+        <v>45902</v>
       </c>
       <c r="I95" s="3">
-        <v>45915</v>
+        <v>45931</v>
       </c>
       <c r="J95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K95" t="s">
         <v>1</v>
       </c>
       <c r="L95" s="3">
-        <v>45891</v>
+        <v>45901</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -4723,22 +4720,22 @@
         <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F96" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G96" s="3">
         <v>45901</v>
       </c>
       <c r="H96" s="3">
-        <v>45902</v>
+        <v>45968</v>
       </c>
       <c r="I96" s="3">
-        <v>45931</v>
+        <v>45993</v>
       </c>
       <c r="J96" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="K96" t="s">
         <v>1</v>
@@ -4752,7 +4749,7 @@
         <v>0</v>
       </c>
       <c r="B97" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C97" s="2">
         <v>1</v>
@@ -4761,22 +4758,22 @@
         <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>4</v>
+        <v>191</v>
       </c>
       <c r="F97" t="s">
-        <v>5</v>
+        <v>192</v>
       </c>
       <c r="G97" s="3">
         <v>45901</v>
       </c>
       <c r="H97" s="3">
-        <v>45968</v>
+        <v>46055</v>
       </c>
       <c r="I97" s="3">
-        <v>45993</v>
+        <v>46140</v>
       </c>
       <c r="J97" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K97" t="s">
         <v>1</v>
@@ -4785,47 +4782,9 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B98" t="s">
-        <v>191</v>
-      </c>
-      <c r="C98" s="2">
-        <v>1</v>
-      </c>
-      <c r="D98" s="2">
-        <v>0</v>
-      </c>
-      <c r="E98" t="s">
-        <v>192</v>
-      </c>
-      <c r="F98" t="s">
-        <v>193</v>
-      </c>
-      <c r="G98" s="3">
-        <v>45901</v>
-      </c>
-      <c r="H98" s="3">
-        <v>46055</v>
-      </c>
-      <c r="I98" s="3">
-        <v>46140</v>
-      </c>
-      <c r="J98" t="s">
-        <v>190</v>
-      </c>
-      <c r="K98" t="s">
-        <v>1</v>
-      </c>
-      <c r="L98" s="3">
-        <v>45901</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L98">
-    <sortCondition ref="B2:B98"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L97">
+    <sortCondition ref="B2:B97"/>
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>